<commit_message>
cambios en el cultivo de la papa (estab repetido)
</commit_message>
<xml_diff>
--- a/Aptitudes_cultivos/data_sipra_normalizado.xlsx
+++ b/Aptitudes_cultivos/data_sipra_normalizado.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J385"/>
+  <dimension ref="A1:J353"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11935,194 +11935,194 @@
     </row>
     <row r="322">
       <c r="A322" s="1" t="n">
-        <v>448</v>
+        <v>480</v>
       </c>
       <c r="B322" t="n">
         <v>0</v>
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>CUNDINAMARCA</t>
+          <t>VICHADA</t>
         </is>
       </c>
       <c r="E322" t="n">
-        <v>265999</v>
+        <v>55220</v>
       </c>
       <c r="F322" t="n">
-        <v>142505</v>
+        <v>753733</v>
       </c>
       <c r="G322" t="n">
-        <v>20141</v>
+        <v>1404817</v>
       </c>
       <c r="H322" t="n">
         <v>0</v>
       </c>
       <c r="I322" t="n">
-        <v>428645</v>
+        <v>2213770</v>
       </c>
       <c r="J322" t="n">
-        <v>2236783</v>
+        <v>10008757</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="n">
-        <v>449</v>
+        <v>481</v>
       </c>
       <c r="B323" t="n">
         <v>1</v>
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>BOYACA</t>
+          <t>META</t>
         </is>
       </c>
       <c r="E323" t="n">
-        <v>261244</v>
+        <v>851481</v>
       </c>
       <c r="F323" t="n">
-        <v>62869</v>
+        <v>833851</v>
       </c>
       <c r="G323" t="n">
-        <v>11640</v>
+        <v>495040</v>
       </c>
       <c r="H323" t="n">
         <v>0</v>
       </c>
       <c r="I323" t="n">
-        <v>335753</v>
+        <v>2180372</v>
       </c>
       <c r="J323" t="n">
-        <v>2317531</v>
+        <v>8555025</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="n">
-        <v>450</v>
+        <v>482</v>
       </c>
       <c r="B324" t="n">
         <v>2</v>
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>NARIÃ‘O</t>
+          <t>ANTIOQUIA</t>
         </is>
       </c>
       <c r="E324" t="n">
-        <v>134353</v>
+        <v>382207</v>
       </c>
       <c r="F324" t="n">
-        <v>52241</v>
+        <v>350531</v>
       </c>
       <c r="G324" t="n">
-        <v>22474</v>
+        <v>320884</v>
       </c>
       <c r="H324" t="n">
         <v>0</v>
       </c>
       <c r="I324" t="n">
-        <v>209068</v>
+        <v>1053622</v>
       </c>
       <c r="J324" t="n">
-        <v>3149751</v>
+        <v>6296299</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="n">
-        <v>451</v>
+        <v>483</v>
       </c>
       <c r="B325" t="n">
         <v>3</v>
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>CAUCA</t>
+          <t>CAQUETA</t>
         </is>
       </c>
       <c r="E325" t="n">
-        <v>37813</v>
+        <v>142662</v>
       </c>
       <c r="F325" t="n">
-        <v>76666</v>
+        <v>482739</v>
       </c>
       <c r="G325" t="n">
-        <v>62846</v>
+        <v>400643</v>
       </c>
       <c r="H325" t="n">
         <v>0</v>
       </c>
       <c r="I325" t="n">
-        <v>177325</v>
+        <v>1026044</v>
       </c>
       <c r="J325" t="n">
-        <v>3125130</v>
+        <v>9010823</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="n">
-        <v>452</v>
+        <v>484</v>
       </c>
       <c r="B326" t="n">
         <v>4</v>
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>ANTIOQUIA</t>
+          <t>CORDOBA</t>
         </is>
       </c>
       <c r="E326" t="n">
-        <v>105253</v>
+        <v>625495</v>
       </c>
       <c r="F326" t="n">
-        <v>53151</v>
+        <v>140341</v>
       </c>
       <c r="G326" t="n">
-        <v>13660</v>
+        <v>232895</v>
       </c>
       <c r="H326" t="n">
         <v>0</v>
       </c>
       <c r="I326" t="n">
-        <v>172064</v>
+        <v>998731</v>
       </c>
       <c r="J326" t="n">
-        <v>6296299</v>
+        <v>2499858</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="n">
-        <v>453</v>
+        <v>485</v>
       </c>
       <c r="B327" t="n">
         <v>5</v>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D327" t="inlineStr">
@@ -12131,19 +12131,19 @@
         </is>
       </c>
       <c r="E327" t="n">
-        <v>26202</v>
+        <v>168634</v>
       </c>
       <c r="F327" t="n">
-        <v>61036</v>
+        <v>207697</v>
       </c>
       <c r="G327" t="n">
-        <v>14493</v>
+        <v>227217</v>
       </c>
       <c r="H327" t="n">
         <v>0</v>
       </c>
       <c r="I327" t="n">
-        <v>101731</v>
+        <v>603548</v>
       </c>
       <c r="J327" t="n">
         <v>3054326</v>
@@ -12151,338 +12151,338 @@
     </row>
     <row r="328">
       <c r="A328" s="1" t="n">
-        <v>454</v>
+        <v>486</v>
       </c>
       <c r="B328" t="n">
         <v>6</v>
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>TOLIMA</t>
+          <t>CESAR</t>
         </is>
       </c>
       <c r="E328" t="n">
-        <v>16740</v>
+        <v>281310</v>
       </c>
       <c r="F328" t="n">
-        <v>32569</v>
+        <v>185287</v>
       </c>
       <c r="G328" t="n">
-        <v>21049</v>
+        <v>84267</v>
       </c>
       <c r="H328" t="n">
         <v>0</v>
       </c>
       <c r="I328" t="n">
-        <v>70358</v>
+        <v>550864</v>
       </c>
       <c r="J328" t="n">
-        <v>2415020</v>
+        <v>2256550</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="n">
-        <v>455</v>
+        <v>487</v>
       </c>
       <c r="B329" t="n">
         <v>7</v>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>CALDAS</t>
+          <t>BOLIVAR</t>
         </is>
       </c>
       <c r="E329" t="n">
-        <v>1571</v>
+        <v>135987</v>
       </c>
       <c r="F329" t="n">
-        <v>30035</v>
+        <v>163286</v>
       </c>
       <c r="G329" t="n">
-        <v>27655</v>
+        <v>175415</v>
       </c>
       <c r="H329" t="n">
         <v>0</v>
       </c>
       <c r="I329" t="n">
-        <v>59261</v>
+        <v>474688</v>
       </c>
       <c r="J329" t="n">
-        <v>743890</v>
+        <v>2665496</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="1" t="n">
-        <v>456</v>
+        <v>488</v>
       </c>
       <c r="B330" t="n">
         <v>8</v>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>NORTE DE SANTANDER</t>
+          <t>MAGDALENA</t>
         </is>
       </c>
       <c r="E330" t="n">
-        <v>21917</v>
+        <v>221244</v>
       </c>
       <c r="F330" t="n">
-        <v>27608</v>
+        <v>128326</v>
       </c>
       <c r="G330" t="n">
-        <v>8538</v>
+        <v>91347</v>
       </c>
       <c r="H330" t="n">
         <v>0</v>
       </c>
       <c r="I330" t="n">
-        <v>58063</v>
+        <v>440917</v>
       </c>
       <c r="J330" t="n">
-        <v>2182705</v>
+        <v>2314438</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="1" t="n">
-        <v>457</v>
+        <v>489</v>
       </c>
       <c r="B331" t="n">
         <v>9</v>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>VALLE DEL CAUCA</t>
+          <t>TOLIMA</t>
         </is>
       </c>
       <c r="E331" t="n">
-        <v>23363</v>
+        <v>96922</v>
       </c>
       <c r="F331" t="n">
-        <v>5976</v>
+        <v>132544</v>
       </c>
       <c r="G331" t="n">
-        <v>3068</v>
+        <v>161564</v>
       </c>
       <c r="H331" t="n">
         <v>0</v>
       </c>
       <c r="I331" t="n">
-        <v>32407</v>
+        <v>391030</v>
       </c>
       <c r="J331" t="n">
-        <v>2076805</v>
+        <v>2415020</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="1" t="n">
-        <v>458</v>
+        <v>490</v>
       </c>
       <c r="B332" t="n">
         <v>10</v>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>PUTUMAYO</t>
+          <t>HUILA</t>
         </is>
       </c>
       <c r="E332" t="n">
-        <v>0</v>
+        <v>38176</v>
       </c>
       <c r="F332" t="n">
-        <v>8110</v>
+        <v>135727</v>
       </c>
       <c r="G332" t="n">
-        <v>6297</v>
+        <v>130175</v>
       </c>
       <c r="H332" t="n">
         <v>0</v>
       </c>
       <c r="I332" t="n">
-        <v>14408</v>
+        <v>304078</v>
       </c>
       <c r="J332" t="n">
-        <v>2584632</v>
+        <v>1813533</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="1" t="n">
-        <v>459</v>
+        <v>491</v>
       </c>
       <c r="B333" t="n">
         <v>11</v>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>HUILA</t>
+          <t>CUNDINAMARCA</t>
         </is>
       </c>
       <c r="E333" t="n">
-        <v>705</v>
+        <v>129648</v>
       </c>
       <c r="F333" t="n">
-        <v>4135</v>
+        <v>83360</v>
       </c>
       <c r="G333" t="n">
-        <v>5317</v>
+        <v>68966</v>
       </c>
       <c r="H333" t="n">
         <v>0</v>
       </c>
       <c r="I333" t="n">
-        <v>10157</v>
+        <v>281974</v>
       </c>
       <c r="J333" t="n">
-        <v>1813533</v>
+        <v>2236783</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="1" t="n">
-        <v>460</v>
+        <v>492</v>
       </c>
       <c r="B334" t="n">
         <v>12</v>
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D334" t="inlineStr">
         <is>
-          <t>QUINDIO</t>
+          <t>SUCRE</t>
         </is>
       </c>
       <c r="E334" t="n">
-        <v>0</v>
+        <v>242085</v>
       </c>
       <c r="F334" t="n">
-        <v>321</v>
+        <v>37130</v>
       </c>
       <c r="G334" t="n">
-        <v>5081</v>
+        <v>2649</v>
       </c>
       <c r="H334" t="n">
         <v>0</v>
       </c>
       <c r="I334" t="n">
-        <v>5402</v>
+        <v>281864</v>
       </c>
       <c r="J334" t="n">
-        <v>193217</v>
+        <v>1071860</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="1" t="n">
-        <v>461</v>
+        <v>493</v>
       </c>
       <c r="B335" t="n">
         <v>13</v>
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D335" t="inlineStr">
         <is>
-          <t>RISARALDA</t>
+          <t>CAUCA</t>
         </is>
       </c>
       <c r="E335" t="n">
-        <v>2536</v>
+        <v>102393</v>
       </c>
       <c r="F335" t="n">
-        <v>769</v>
+        <v>96605</v>
       </c>
       <c r="G335" t="n">
-        <v>88</v>
+        <v>78155</v>
       </c>
       <c r="H335" t="n">
         <v>0</v>
       </c>
       <c r="I335" t="n">
-        <v>3393</v>
+        <v>277153</v>
       </c>
       <c r="J335" t="n">
-        <v>356035</v>
+        <v>3125130</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="1" t="n">
-        <v>462</v>
+        <v>494</v>
       </c>
       <c r="B336" t="n">
         <v>14</v>
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D336" t="inlineStr">
         <is>
-          <t>META</t>
+          <t>VALLE DEL CAUCA</t>
         </is>
       </c>
       <c r="E336" t="n">
-        <v>0</v>
+        <v>143394</v>
       </c>
       <c r="F336" t="n">
-        <v>152</v>
+        <v>125435</v>
       </c>
       <c r="G336" t="n">
-        <v>255</v>
+        <v>4074</v>
       </c>
       <c r="H336" t="n">
         <v>0</v>
       </c>
       <c r="I336" t="n">
-        <v>407</v>
+        <v>272903</v>
       </c>
       <c r="J336" t="n">
-        <v>8555025</v>
+        <v>2076805</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="1" t="n">
-        <v>463</v>
+        <v>495</v>
       </c>
       <c r="B337" t="n">
         <v>15</v>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D337" t="inlineStr">
@@ -12491,19 +12491,19 @@
         </is>
       </c>
       <c r="E337" t="n">
-        <v>0</v>
+        <v>185992</v>
       </c>
       <c r="F337" t="n">
-        <v>0</v>
+        <v>46093</v>
       </c>
       <c r="G337" t="n">
-        <v>166</v>
+        <v>39203</v>
       </c>
       <c r="H337" t="n">
         <v>0</v>
       </c>
       <c r="I337" t="n">
-        <v>166</v>
+        <v>271289</v>
       </c>
       <c r="J337" t="n">
         <v>4434139</v>
@@ -12511,194 +12511,194 @@
     </row>
     <row r="338">
       <c r="A338" s="1" t="n">
-        <v>464</v>
+        <v>496</v>
       </c>
       <c r="B338" t="n">
         <v>16</v>
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D338" t="inlineStr">
         <is>
-          <t>CESAR</t>
+          <t>LA GUAJIRA</t>
         </is>
       </c>
       <c r="E338" t="n">
-        <v>0</v>
+        <v>65543</v>
       </c>
       <c r="F338" t="n">
-        <v>45</v>
+        <v>78630</v>
       </c>
       <c r="G338" t="n">
-        <v>52</v>
+        <v>38872</v>
       </c>
       <c r="H338" t="n">
         <v>0</v>
       </c>
       <c r="I338" t="n">
-        <v>97</v>
+        <v>183045</v>
       </c>
       <c r="J338" t="n">
-        <v>2256550</v>
+        <v>2061936</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="1" t="n">
-        <v>465</v>
+        <v>497</v>
       </c>
       <c r="B339" t="n">
         <v>17</v>
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D339" t="inlineStr">
         <is>
-          <t>MAGDALENA</t>
+          <t>PUTUMAYO</t>
         </is>
       </c>
       <c r="E339" t="n">
-        <v>0</v>
+        <v>2427</v>
       </c>
       <c r="F339" t="n">
-        <v>0</v>
+        <v>6372</v>
       </c>
       <c r="G339" t="n">
-        <v>38</v>
+        <v>173825</v>
       </c>
       <c r="H339" t="n">
         <v>0</v>
       </c>
       <c r="I339" t="n">
-        <v>38</v>
+        <v>182624</v>
       </c>
       <c r="J339" t="n">
-        <v>2314438</v>
+        <v>2584632</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="1" t="n">
-        <v>466</v>
+        <v>498</v>
       </c>
       <c r="B340" t="n">
         <v>18</v>
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D340" t="inlineStr">
         <is>
-          <t>CAQUETA</t>
+          <t>GUAVIARE</t>
         </is>
       </c>
       <c r="E340" t="n">
-        <v>0</v>
+        <v>886</v>
       </c>
       <c r="F340" t="n">
-        <v>0</v>
+        <v>91161</v>
       </c>
       <c r="G340" t="n">
-        <v>0</v>
+        <v>77624</v>
       </c>
       <c r="H340" t="n">
         <v>0</v>
       </c>
       <c r="I340" t="n">
-        <v>0</v>
+        <v>169671</v>
       </c>
       <c r="J340" t="n">
-        <v>9010823</v>
+        <v>5557912</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="1" t="n">
-        <v>467</v>
+        <v>499</v>
       </c>
       <c r="B341" t="n">
         <v>19</v>
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D341" t="inlineStr">
         <is>
-          <t>BOLIVAR</t>
+          <t>NORTE DE SANTANDER</t>
         </is>
       </c>
       <c r="E341" t="n">
-        <v>0</v>
+        <v>57293</v>
       </c>
       <c r="F341" t="n">
-        <v>0</v>
+        <v>35184</v>
       </c>
       <c r="G341" t="n">
-        <v>0</v>
+        <v>46556</v>
       </c>
       <c r="H341" t="n">
         <v>0</v>
       </c>
       <c r="I341" t="n">
-        <v>0</v>
+        <v>139033</v>
       </c>
       <c r="J341" t="n">
-        <v>2665496</v>
+        <v>2182705</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="1" t="n">
-        <v>468</v>
+        <v>500</v>
       </c>
       <c r="B342" t="n">
         <v>20</v>
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D342" t="inlineStr">
         <is>
-          <t>SUCRE</t>
+          <t>CALDAS</t>
         </is>
       </c>
       <c r="E342" t="n">
-        <v>0</v>
+        <v>49686</v>
       </c>
       <c r="F342" t="n">
-        <v>0</v>
+        <v>51908</v>
       </c>
       <c r="G342" t="n">
-        <v>0</v>
+        <v>32838</v>
       </c>
       <c r="H342" t="n">
         <v>0</v>
       </c>
       <c r="I342" t="n">
-        <v>0</v>
+        <v>134432</v>
       </c>
       <c r="J342" t="n">
-        <v>1071860</v>
+        <v>743890</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="1" t="n">
-        <v>469</v>
+        <v>501</v>
       </c>
       <c r="B343" t="n">
         <v>21</v>
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D343" t="inlineStr">
@@ -12707,19 +12707,19 @@
         </is>
       </c>
       <c r="E343" t="n">
-        <v>0</v>
+        <v>35157</v>
       </c>
       <c r="F343" t="n">
-        <v>0</v>
+        <v>74973</v>
       </c>
       <c r="G343" t="n">
-        <v>0</v>
+        <v>18938</v>
       </c>
       <c r="H343" t="n">
         <v>0</v>
       </c>
       <c r="I343" t="n">
-        <v>0</v>
+        <v>129068</v>
       </c>
       <c r="J343" t="n">
         <v>331159</v>
@@ -12727,134 +12727,134 @@
     </row>
     <row r="344">
       <c r="A344" s="1" t="n">
-        <v>470</v>
+        <v>502</v>
       </c>
       <c r="B344" t="n">
         <v>22</v>
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D344" t="inlineStr">
         <is>
-          <t>ARAUCA</t>
+          <t>BOYACA</t>
         </is>
       </c>
       <c r="E344" t="n">
-        <v>0</v>
+        <v>72015</v>
       </c>
       <c r="F344" t="n">
-        <v>0</v>
+        <v>25647</v>
       </c>
       <c r="G344" t="n">
-        <v>0</v>
+        <v>30754</v>
       </c>
       <c r="H344" t="n">
         <v>0</v>
       </c>
       <c r="I344" t="n">
-        <v>0</v>
+        <v>128416</v>
       </c>
       <c r="J344" t="n">
-        <v>2383135</v>
+        <v>2317531</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="1" t="n">
-        <v>471</v>
+        <v>503</v>
       </c>
       <c r="B345" t="n">
         <v>23</v>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D345" t="inlineStr">
         <is>
-          <t>ARCHIPIELAGO DE SAN ANDRES PROVIDENCIA Y SANTA CATALINA</t>
+          <t>NARIÃ‘O</t>
         </is>
       </c>
       <c r="E345" t="n">
-        <v>0</v>
+        <v>19944</v>
       </c>
       <c r="F345" t="n">
-        <v>0</v>
+        <v>45342</v>
       </c>
       <c r="G345" t="n">
-        <v>0</v>
+        <v>46167</v>
       </c>
       <c r="H345" t="n">
         <v>0</v>
       </c>
       <c r="I345" t="n">
-        <v>0</v>
+        <v>111453</v>
       </c>
       <c r="J345" t="n">
-        <v>4972</v>
+        <v>3149751</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="1" t="n">
-        <v>472</v>
+        <v>504</v>
       </c>
       <c r="B346" t="n">
         <v>24</v>
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D346" t="inlineStr">
         <is>
-          <t>AMAZONAS</t>
+          <t>CHOCO</t>
         </is>
       </c>
       <c r="E346" t="n">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="F346" t="n">
-        <v>0</v>
+        <v>16077</v>
       </c>
       <c r="G346" t="n">
-        <v>0</v>
+        <v>66550</v>
       </c>
       <c r="H346" t="n">
         <v>0</v>
       </c>
       <c r="I346" t="n">
-        <v>0</v>
+        <v>82715</v>
       </c>
       <c r="J346" t="n">
-        <v>10903686</v>
+        <v>4824344</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="1" t="n">
-        <v>473</v>
+        <v>505</v>
       </c>
       <c r="B347" t="n">
         <v>25</v>
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D347" t="inlineStr">
         <is>
-          <t>GUAINIA</t>
+          <t>ARAUCA</t>
         </is>
       </c>
       <c r="E347" t="n">
-        <v>0</v>
+        <v>63048</v>
       </c>
       <c r="F347" t="n">
-        <v>0</v>
+        <v>762</v>
       </c>
       <c r="G347" t="n">
         <v>0</v>
@@ -12863,70 +12863,70 @@
         <v>0</v>
       </c>
       <c r="I347" t="n">
-        <v>0</v>
+        <v>63810</v>
       </c>
       <c r="J347" t="n">
-        <v>7140386</v>
+        <v>2383135</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="1" t="n">
-        <v>474</v>
+        <v>506</v>
       </c>
       <c r="B348" t="n">
         <v>26</v>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D348" t="inlineStr">
         <is>
-          <t>GUAVIARE</t>
+          <t>RISARALDA</t>
         </is>
       </c>
       <c r="E348" t="n">
-        <v>0</v>
+        <v>21497</v>
       </c>
       <c r="F348" t="n">
-        <v>0</v>
+        <v>18743</v>
       </c>
       <c r="G348" t="n">
-        <v>0</v>
+        <v>20350</v>
       </c>
       <c r="H348" t="n">
         <v>0</v>
       </c>
       <c r="I348" t="n">
-        <v>0</v>
+        <v>60590</v>
       </c>
       <c r="J348" t="n">
-        <v>5557912</v>
+        <v>356035</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="1" t="n">
-        <v>475</v>
+        <v>507</v>
       </c>
       <c r="B349" t="n">
         <v>27</v>
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D349" t="inlineStr">
         <is>
-          <t>VAUPES</t>
+          <t>QUINDIO</t>
         </is>
       </c>
       <c r="E349" t="n">
-        <v>0</v>
+        <v>47444</v>
       </c>
       <c r="F349" t="n">
-        <v>0</v>
+        <v>6667</v>
       </c>
       <c r="G349" t="n">
         <v>0</v>
@@ -12935,99 +12935,99 @@
         <v>0</v>
       </c>
       <c r="I349" t="n">
-        <v>0</v>
+        <v>54112</v>
       </c>
       <c r="J349" t="n">
-        <v>5343179</v>
+        <v>193217</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="1" t="n">
-        <v>476</v>
+        <v>508</v>
       </c>
       <c r="B350" t="n">
         <v>28</v>
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D350" t="inlineStr">
         <is>
-          <t>CORDOBA</t>
+          <t>AMAZONAS</t>
         </is>
       </c>
       <c r="E350" t="n">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="F350" t="n">
-        <v>0</v>
+        <v>1182</v>
       </c>
       <c r="G350" t="n">
-        <v>0</v>
+        <v>11069</v>
       </c>
       <c r="H350" t="n">
         <v>0</v>
       </c>
       <c r="I350" t="n">
-        <v>0</v>
+        <v>12344</v>
       </c>
       <c r="J350" t="n">
-        <v>2499858</v>
+        <v>10903686</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="1" t="n">
-        <v>477</v>
+        <v>509</v>
       </c>
       <c r="B351" t="n">
         <v>29</v>
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D351" t="inlineStr">
         <is>
-          <t>VICHADA</t>
+          <t>GUAINIA</t>
         </is>
       </c>
       <c r="E351" t="n">
         <v>0</v>
       </c>
       <c r="F351" t="n">
-        <v>0</v>
+        <v>3060</v>
       </c>
       <c r="G351" t="n">
-        <v>0</v>
+        <v>8631</v>
       </c>
       <c r="H351" t="n">
         <v>0</v>
       </c>
       <c r="I351" t="n">
-        <v>0</v>
+        <v>11691</v>
       </c>
       <c r="J351" t="n">
-        <v>10008757</v>
+        <v>7140386</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="1" t="n">
-        <v>478</v>
+        <v>510</v>
       </c>
       <c r="B352" t="n">
         <v>30</v>
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D352" t="inlineStr">
         <is>
-          <t>CHOCO</t>
+          <t>VAUPES</t>
         </is>
       </c>
       <c r="E352" t="n">
@@ -13037,33 +13037,33 @@
         <v>0</v>
       </c>
       <c r="G352" t="n">
-        <v>0</v>
+        <v>6844</v>
       </c>
       <c r="H352" t="n">
         <v>0</v>
       </c>
       <c r="I352" t="n">
-        <v>0</v>
+        <v>6844</v>
       </c>
       <c r="J352" t="n">
-        <v>4824344</v>
+        <v>5343179</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="1" t="n">
-        <v>479</v>
+        <v>511</v>
       </c>
       <c r="B353" t="n">
         <v>31</v>
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>PAPA</t>
+          <t>PAPAYA</t>
         </is>
       </c>
       <c r="D353" t="inlineStr">
         <is>
-          <t>LA GUAJIRA</t>
+          <t>ARCHIPIELAGO DE SAN ANDRES PROVIDENCIA Y SANTA CATALINA</t>
         </is>
       </c>
       <c r="E353" t="n">
@@ -13082,1158 +13082,6 @@
         <v>0</v>
       </c>
       <c r="J353" t="n">
-        <v>2061936</v>
-      </c>
-    </row>
-    <row r="354">
-      <c r="A354" s="1" t="n">
-        <v>480</v>
-      </c>
-      <c r="B354" t="n">
-        <v>0</v>
-      </c>
-      <c r="C354" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D354" t="inlineStr">
-        <is>
-          <t>VICHADA</t>
-        </is>
-      </c>
-      <c r="E354" t="n">
-        <v>55220</v>
-      </c>
-      <c r="F354" t="n">
-        <v>753733</v>
-      </c>
-      <c r="G354" t="n">
-        <v>1404817</v>
-      </c>
-      <c r="H354" t="n">
-        <v>0</v>
-      </c>
-      <c r="I354" t="n">
-        <v>2213770</v>
-      </c>
-      <c r="J354" t="n">
-        <v>10008757</v>
-      </c>
-    </row>
-    <row r="355">
-      <c r="A355" s="1" t="n">
-        <v>481</v>
-      </c>
-      <c r="B355" t="n">
-        <v>1</v>
-      </c>
-      <c r="C355" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D355" t="inlineStr">
-        <is>
-          <t>META</t>
-        </is>
-      </c>
-      <c r="E355" t="n">
-        <v>851481</v>
-      </c>
-      <c r="F355" t="n">
-        <v>833851</v>
-      </c>
-      <c r="G355" t="n">
-        <v>495040</v>
-      </c>
-      <c r="H355" t="n">
-        <v>0</v>
-      </c>
-      <c r="I355" t="n">
-        <v>2180372</v>
-      </c>
-      <c r="J355" t="n">
-        <v>8555025</v>
-      </c>
-    </row>
-    <row r="356">
-      <c r="A356" s="1" t="n">
-        <v>482</v>
-      </c>
-      <c r="B356" t="n">
-        <v>2</v>
-      </c>
-      <c r="C356" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D356" t="inlineStr">
-        <is>
-          <t>ANTIOQUIA</t>
-        </is>
-      </c>
-      <c r="E356" t="n">
-        <v>382207</v>
-      </c>
-      <c r="F356" t="n">
-        <v>350531</v>
-      </c>
-      <c r="G356" t="n">
-        <v>320884</v>
-      </c>
-      <c r="H356" t="n">
-        <v>0</v>
-      </c>
-      <c r="I356" t="n">
-        <v>1053622</v>
-      </c>
-      <c r="J356" t="n">
-        <v>6296299</v>
-      </c>
-    </row>
-    <row r="357">
-      <c r="A357" s="1" t="n">
-        <v>483</v>
-      </c>
-      <c r="B357" t="n">
-        <v>3</v>
-      </c>
-      <c r="C357" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D357" t="inlineStr">
-        <is>
-          <t>CAQUETA</t>
-        </is>
-      </c>
-      <c r="E357" t="n">
-        <v>142662</v>
-      </c>
-      <c r="F357" t="n">
-        <v>482739</v>
-      </c>
-      <c r="G357" t="n">
-        <v>400643</v>
-      </c>
-      <c r="H357" t="n">
-        <v>0</v>
-      </c>
-      <c r="I357" t="n">
-        <v>1026044</v>
-      </c>
-      <c r="J357" t="n">
-        <v>9010823</v>
-      </c>
-    </row>
-    <row r="358">
-      <c r="A358" s="1" t="n">
-        <v>484</v>
-      </c>
-      <c r="B358" t="n">
-        <v>4</v>
-      </c>
-      <c r="C358" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D358" t="inlineStr">
-        <is>
-          <t>CORDOBA</t>
-        </is>
-      </c>
-      <c r="E358" t="n">
-        <v>625495</v>
-      </c>
-      <c r="F358" t="n">
-        <v>140341</v>
-      </c>
-      <c r="G358" t="n">
-        <v>232895</v>
-      </c>
-      <c r="H358" t="n">
-        <v>0</v>
-      </c>
-      <c r="I358" t="n">
-        <v>998731</v>
-      </c>
-      <c r="J358" t="n">
-        <v>2499858</v>
-      </c>
-    </row>
-    <row r="359">
-      <c r="A359" s="1" t="n">
-        <v>485</v>
-      </c>
-      <c r="B359" t="n">
-        <v>5</v>
-      </c>
-      <c r="C359" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D359" t="inlineStr">
-        <is>
-          <t>SANTANDER</t>
-        </is>
-      </c>
-      <c r="E359" t="n">
-        <v>168634</v>
-      </c>
-      <c r="F359" t="n">
-        <v>207697</v>
-      </c>
-      <c r="G359" t="n">
-        <v>227217</v>
-      </c>
-      <c r="H359" t="n">
-        <v>0</v>
-      </c>
-      <c r="I359" t="n">
-        <v>603548</v>
-      </c>
-      <c r="J359" t="n">
-        <v>3054326</v>
-      </c>
-    </row>
-    <row r="360">
-      <c r="A360" s="1" t="n">
-        <v>486</v>
-      </c>
-      <c r="B360" t="n">
-        <v>6</v>
-      </c>
-      <c r="C360" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D360" t="inlineStr">
-        <is>
-          <t>CESAR</t>
-        </is>
-      </c>
-      <c r="E360" t="n">
-        <v>281310</v>
-      </c>
-      <c r="F360" t="n">
-        <v>185287</v>
-      </c>
-      <c r="G360" t="n">
-        <v>84267</v>
-      </c>
-      <c r="H360" t="n">
-        <v>0</v>
-      </c>
-      <c r="I360" t="n">
-        <v>550864</v>
-      </c>
-      <c r="J360" t="n">
-        <v>2256550</v>
-      </c>
-    </row>
-    <row r="361">
-      <c r="A361" s="1" t="n">
-        <v>487</v>
-      </c>
-      <c r="B361" t="n">
-        <v>7</v>
-      </c>
-      <c r="C361" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D361" t="inlineStr">
-        <is>
-          <t>BOLIVAR</t>
-        </is>
-      </c>
-      <c r="E361" t="n">
-        <v>135987</v>
-      </c>
-      <c r="F361" t="n">
-        <v>163286</v>
-      </c>
-      <c r="G361" t="n">
-        <v>175415</v>
-      </c>
-      <c r="H361" t="n">
-        <v>0</v>
-      </c>
-      <c r="I361" t="n">
-        <v>474688</v>
-      </c>
-      <c r="J361" t="n">
-        <v>2665496</v>
-      </c>
-    </row>
-    <row r="362">
-      <c r="A362" s="1" t="n">
-        <v>488</v>
-      </c>
-      <c r="B362" t="n">
-        <v>8</v>
-      </c>
-      <c r="C362" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D362" t="inlineStr">
-        <is>
-          <t>MAGDALENA</t>
-        </is>
-      </c>
-      <c r="E362" t="n">
-        <v>221244</v>
-      </c>
-      <c r="F362" t="n">
-        <v>128326</v>
-      </c>
-      <c r="G362" t="n">
-        <v>91347</v>
-      </c>
-      <c r="H362" t="n">
-        <v>0</v>
-      </c>
-      <c r="I362" t="n">
-        <v>440917</v>
-      </c>
-      <c r="J362" t="n">
-        <v>2314438</v>
-      </c>
-    </row>
-    <row r="363">
-      <c r="A363" s="1" t="n">
-        <v>489</v>
-      </c>
-      <c r="B363" t="n">
-        <v>9</v>
-      </c>
-      <c r="C363" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D363" t="inlineStr">
-        <is>
-          <t>TOLIMA</t>
-        </is>
-      </c>
-      <c r="E363" t="n">
-        <v>96922</v>
-      </c>
-      <c r="F363" t="n">
-        <v>132544</v>
-      </c>
-      <c r="G363" t="n">
-        <v>161564</v>
-      </c>
-      <c r="H363" t="n">
-        <v>0</v>
-      </c>
-      <c r="I363" t="n">
-        <v>391030</v>
-      </c>
-      <c r="J363" t="n">
-        <v>2415020</v>
-      </c>
-    </row>
-    <row r="364">
-      <c r="A364" s="1" t="n">
-        <v>490</v>
-      </c>
-      <c r="B364" t="n">
-        <v>10</v>
-      </c>
-      <c r="C364" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D364" t="inlineStr">
-        <is>
-          <t>HUILA</t>
-        </is>
-      </c>
-      <c r="E364" t="n">
-        <v>38176</v>
-      </c>
-      <c r="F364" t="n">
-        <v>135727</v>
-      </c>
-      <c r="G364" t="n">
-        <v>130175</v>
-      </c>
-      <c r="H364" t="n">
-        <v>0</v>
-      </c>
-      <c r="I364" t="n">
-        <v>304078</v>
-      </c>
-      <c r="J364" t="n">
-        <v>1813533</v>
-      </c>
-    </row>
-    <row r="365">
-      <c r="A365" s="1" t="n">
-        <v>491</v>
-      </c>
-      <c r="B365" t="n">
-        <v>11</v>
-      </c>
-      <c r="C365" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D365" t="inlineStr">
-        <is>
-          <t>CUNDINAMARCA</t>
-        </is>
-      </c>
-      <c r="E365" t="n">
-        <v>129648</v>
-      </c>
-      <c r="F365" t="n">
-        <v>83360</v>
-      </c>
-      <c r="G365" t="n">
-        <v>68966</v>
-      </c>
-      <c r="H365" t="n">
-        <v>0</v>
-      </c>
-      <c r="I365" t="n">
-        <v>281974</v>
-      </c>
-      <c r="J365" t="n">
-        <v>2236783</v>
-      </c>
-    </row>
-    <row r="366">
-      <c r="A366" s="1" t="n">
-        <v>492</v>
-      </c>
-      <c r="B366" t="n">
-        <v>12</v>
-      </c>
-      <c r="C366" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D366" t="inlineStr">
-        <is>
-          <t>SUCRE</t>
-        </is>
-      </c>
-      <c r="E366" t="n">
-        <v>242085</v>
-      </c>
-      <c r="F366" t="n">
-        <v>37130</v>
-      </c>
-      <c r="G366" t="n">
-        <v>2649</v>
-      </c>
-      <c r="H366" t="n">
-        <v>0</v>
-      </c>
-      <c r="I366" t="n">
-        <v>281864</v>
-      </c>
-      <c r="J366" t="n">
-        <v>1071860</v>
-      </c>
-    </row>
-    <row r="367">
-      <c r="A367" s="1" t="n">
-        <v>493</v>
-      </c>
-      <c r="B367" t="n">
-        <v>13</v>
-      </c>
-      <c r="C367" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D367" t="inlineStr">
-        <is>
-          <t>CAUCA</t>
-        </is>
-      </c>
-      <c r="E367" t="n">
-        <v>102393</v>
-      </c>
-      <c r="F367" t="n">
-        <v>96605</v>
-      </c>
-      <c r="G367" t="n">
-        <v>78155</v>
-      </c>
-      <c r="H367" t="n">
-        <v>0</v>
-      </c>
-      <c r="I367" t="n">
-        <v>277153</v>
-      </c>
-      <c r="J367" t="n">
-        <v>3125130</v>
-      </c>
-    </row>
-    <row r="368">
-      <c r="A368" s="1" t="n">
-        <v>494</v>
-      </c>
-      <c r="B368" t="n">
-        <v>14</v>
-      </c>
-      <c r="C368" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D368" t="inlineStr">
-        <is>
-          <t>VALLE DEL CAUCA</t>
-        </is>
-      </c>
-      <c r="E368" t="n">
-        <v>143394</v>
-      </c>
-      <c r="F368" t="n">
-        <v>125435</v>
-      </c>
-      <c r="G368" t="n">
-        <v>4074</v>
-      </c>
-      <c r="H368" t="n">
-        <v>0</v>
-      </c>
-      <c r="I368" t="n">
-        <v>272903</v>
-      </c>
-      <c r="J368" t="n">
-        <v>2076805</v>
-      </c>
-    </row>
-    <row r="369">
-      <c r="A369" s="1" t="n">
-        <v>495</v>
-      </c>
-      <c r="B369" t="n">
-        <v>15</v>
-      </c>
-      <c r="C369" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D369" t="inlineStr">
-        <is>
-          <t>CASANARE</t>
-        </is>
-      </c>
-      <c r="E369" t="n">
-        <v>185992</v>
-      </c>
-      <c r="F369" t="n">
-        <v>46093</v>
-      </c>
-      <c r="G369" t="n">
-        <v>39203</v>
-      </c>
-      <c r="H369" t="n">
-        <v>0</v>
-      </c>
-      <c r="I369" t="n">
-        <v>271289</v>
-      </c>
-      <c r="J369" t="n">
-        <v>4434139</v>
-      </c>
-    </row>
-    <row r="370">
-      <c r="A370" s="1" t="n">
-        <v>496</v>
-      </c>
-      <c r="B370" t="n">
-        <v>16</v>
-      </c>
-      <c r="C370" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D370" t="inlineStr">
-        <is>
-          <t>LA GUAJIRA</t>
-        </is>
-      </c>
-      <c r="E370" t="n">
-        <v>65543</v>
-      </c>
-      <c r="F370" t="n">
-        <v>78630</v>
-      </c>
-      <c r="G370" t="n">
-        <v>38872</v>
-      </c>
-      <c r="H370" t="n">
-        <v>0</v>
-      </c>
-      <c r="I370" t="n">
-        <v>183045</v>
-      </c>
-      <c r="J370" t="n">
-        <v>2061936</v>
-      </c>
-    </row>
-    <row r="371">
-      <c r="A371" s="1" t="n">
-        <v>497</v>
-      </c>
-      <c r="B371" t="n">
-        <v>17</v>
-      </c>
-      <c r="C371" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D371" t="inlineStr">
-        <is>
-          <t>PUTUMAYO</t>
-        </is>
-      </c>
-      <c r="E371" t="n">
-        <v>2427</v>
-      </c>
-      <c r="F371" t="n">
-        <v>6372</v>
-      </c>
-      <c r="G371" t="n">
-        <v>173825</v>
-      </c>
-      <c r="H371" t="n">
-        <v>0</v>
-      </c>
-      <c r="I371" t="n">
-        <v>182624</v>
-      </c>
-      <c r="J371" t="n">
-        <v>2584632</v>
-      </c>
-    </row>
-    <row r="372">
-      <c r="A372" s="1" t="n">
-        <v>498</v>
-      </c>
-      <c r="B372" t="n">
-        <v>18</v>
-      </c>
-      <c r="C372" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D372" t="inlineStr">
-        <is>
-          <t>GUAVIARE</t>
-        </is>
-      </c>
-      <c r="E372" t="n">
-        <v>886</v>
-      </c>
-      <c r="F372" t="n">
-        <v>91161</v>
-      </c>
-      <c r="G372" t="n">
-        <v>77624</v>
-      </c>
-      <c r="H372" t="n">
-        <v>0</v>
-      </c>
-      <c r="I372" t="n">
-        <v>169671</v>
-      </c>
-      <c r="J372" t="n">
-        <v>5557912</v>
-      </c>
-    </row>
-    <row r="373">
-      <c r="A373" s="1" t="n">
-        <v>499</v>
-      </c>
-      <c r="B373" t="n">
-        <v>19</v>
-      </c>
-      <c r="C373" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D373" t="inlineStr">
-        <is>
-          <t>NORTE DE SANTANDER</t>
-        </is>
-      </c>
-      <c r="E373" t="n">
-        <v>57293</v>
-      </c>
-      <c r="F373" t="n">
-        <v>35184</v>
-      </c>
-      <c r="G373" t="n">
-        <v>46556</v>
-      </c>
-      <c r="H373" t="n">
-        <v>0</v>
-      </c>
-      <c r="I373" t="n">
-        <v>139033</v>
-      </c>
-      <c r="J373" t="n">
-        <v>2182705</v>
-      </c>
-    </row>
-    <row r="374">
-      <c r="A374" s="1" t="n">
-        <v>500</v>
-      </c>
-      <c r="B374" t="n">
-        <v>20</v>
-      </c>
-      <c r="C374" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D374" t="inlineStr">
-        <is>
-          <t>CALDAS</t>
-        </is>
-      </c>
-      <c r="E374" t="n">
-        <v>49686</v>
-      </c>
-      <c r="F374" t="n">
-        <v>51908</v>
-      </c>
-      <c r="G374" t="n">
-        <v>32838</v>
-      </c>
-      <c r="H374" t="n">
-        <v>0</v>
-      </c>
-      <c r="I374" t="n">
-        <v>134432</v>
-      </c>
-      <c r="J374" t="n">
-        <v>743890</v>
-      </c>
-    </row>
-    <row r="375">
-      <c r="A375" s="1" t="n">
-        <v>501</v>
-      </c>
-      <c r="B375" t="n">
-        <v>21</v>
-      </c>
-      <c r="C375" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D375" t="inlineStr">
-        <is>
-          <t>ATLANTICO</t>
-        </is>
-      </c>
-      <c r="E375" t="n">
-        <v>35157</v>
-      </c>
-      <c r="F375" t="n">
-        <v>74973</v>
-      </c>
-      <c r="G375" t="n">
-        <v>18938</v>
-      </c>
-      <c r="H375" t="n">
-        <v>0</v>
-      </c>
-      <c r="I375" t="n">
-        <v>129068</v>
-      </c>
-      <c r="J375" t="n">
-        <v>331159</v>
-      </c>
-    </row>
-    <row r="376">
-      <c r="A376" s="1" t="n">
-        <v>502</v>
-      </c>
-      <c r="B376" t="n">
-        <v>22</v>
-      </c>
-      <c r="C376" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D376" t="inlineStr">
-        <is>
-          <t>BOYACA</t>
-        </is>
-      </c>
-      <c r="E376" t="n">
-        <v>72015</v>
-      </c>
-      <c r="F376" t="n">
-        <v>25647</v>
-      </c>
-      <c r="G376" t="n">
-        <v>30754</v>
-      </c>
-      <c r="H376" t="n">
-        <v>0</v>
-      </c>
-      <c r="I376" t="n">
-        <v>128416</v>
-      </c>
-      <c r="J376" t="n">
-        <v>2317531</v>
-      </c>
-    </row>
-    <row r="377">
-      <c r="A377" s="1" t="n">
-        <v>503</v>
-      </c>
-      <c r="B377" t="n">
-        <v>23</v>
-      </c>
-      <c r="C377" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D377" t="inlineStr">
-        <is>
-          <t>NARIÃ‘O</t>
-        </is>
-      </c>
-      <c r="E377" t="n">
-        <v>19944</v>
-      </c>
-      <c r="F377" t="n">
-        <v>45342</v>
-      </c>
-      <c r="G377" t="n">
-        <v>46167</v>
-      </c>
-      <c r="H377" t="n">
-        <v>0</v>
-      </c>
-      <c r="I377" t="n">
-        <v>111453</v>
-      </c>
-      <c r="J377" t="n">
-        <v>3149751</v>
-      </c>
-    </row>
-    <row r="378">
-      <c r="A378" s="1" t="n">
-        <v>504</v>
-      </c>
-      <c r="B378" t="n">
-        <v>24</v>
-      </c>
-      <c r="C378" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D378" t="inlineStr">
-        <is>
-          <t>CHOCO</t>
-        </is>
-      </c>
-      <c r="E378" t="n">
-        <v>88</v>
-      </c>
-      <c r="F378" t="n">
-        <v>16077</v>
-      </c>
-      <c r="G378" t="n">
-        <v>66550</v>
-      </c>
-      <c r="H378" t="n">
-        <v>0</v>
-      </c>
-      <c r="I378" t="n">
-        <v>82715</v>
-      </c>
-      <c r="J378" t="n">
-        <v>4824344</v>
-      </c>
-    </row>
-    <row r="379">
-      <c r="A379" s="1" t="n">
-        <v>505</v>
-      </c>
-      <c r="B379" t="n">
-        <v>25</v>
-      </c>
-      <c r="C379" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D379" t="inlineStr">
-        <is>
-          <t>ARAUCA</t>
-        </is>
-      </c>
-      <c r="E379" t="n">
-        <v>63048</v>
-      </c>
-      <c r="F379" t="n">
-        <v>762</v>
-      </c>
-      <c r="G379" t="n">
-        <v>0</v>
-      </c>
-      <c r="H379" t="n">
-        <v>0</v>
-      </c>
-      <c r="I379" t="n">
-        <v>63810</v>
-      </c>
-      <c r="J379" t="n">
-        <v>2383135</v>
-      </c>
-    </row>
-    <row r="380">
-      <c r="A380" s="1" t="n">
-        <v>506</v>
-      </c>
-      <c r="B380" t="n">
-        <v>26</v>
-      </c>
-      <c r="C380" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D380" t="inlineStr">
-        <is>
-          <t>RISARALDA</t>
-        </is>
-      </c>
-      <c r="E380" t="n">
-        <v>21497</v>
-      </c>
-      <c r="F380" t="n">
-        <v>18743</v>
-      </c>
-      <c r="G380" t="n">
-        <v>20350</v>
-      </c>
-      <c r="H380" t="n">
-        <v>0</v>
-      </c>
-      <c r="I380" t="n">
-        <v>60590</v>
-      </c>
-      <c r="J380" t="n">
-        <v>356035</v>
-      </c>
-    </row>
-    <row r="381">
-      <c r="A381" s="1" t="n">
-        <v>507</v>
-      </c>
-      <c r="B381" t="n">
-        <v>27</v>
-      </c>
-      <c r="C381" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D381" t="inlineStr">
-        <is>
-          <t>QUINDIO</t>
-        </is>
-      </c>
-      <c r="E381" t="n">
-        <v>47444</v>
-      </c>
-      <c r="F381" t="n">
-        <v>6667</v>
-      </c>
-      <c r="G381" t="n">
-        <v>0</v>
-      </c>
-      <c r="H381" t="n">
-        <v>0</v>
-      </c>
-      <c r="I381" t="n">
-        <v>54112</v>
-      </c>
-      <c r="J381" t="n">
-        <v>193217</v>
-      </c>
-    </row>
-    <row r="382">
-      <c r="A382" s="1" t="n">
-        <v>508</v>
-      </c>
-      <c r="B382" t="n">
-        <v>28</v>
-      </c>
-      <c r="C382" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D382" t="inlineStr">
-        <is>
-          <t>AMAZONAS</t>
-        </is>
-      </c>
-      <c r="E382" t="n">
-        <v>93</v>
-      </c>
-      <c r="F382" t="n">
-        <v>1182</v>
-      </c>
-      <c r="G382" t="n">
-        <v>11069</v>
-      </c>
-      <c r="H382" t="n">
-        <v>0</v>
-      </c>
-      <c r="I382" t="n">
-        <v>12344</v>
-      </c>
-      <c r="J382" t="n">
-        <v>10903686</v>
-      </c>
-    </row>
-    <row r="383">
-      <c r="A383" s="1" t="n">
-        <v>509</v>
-      </c>
-      <c r="B383" t="n">
-        <v>29</v>
-      </c>
-      <c r="C383" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D383" t="inlineStr">
-        <is>
-          <t>GUAINIA</t>
-        </is>
-      </c>
-      <c r="E383" t="n">
-        <v>0</v>
-      </c>
-      <c r="F383" t="n">
-        <v>3060</v>
-      </c>
-      <c r="G383" t="n">
-        <v>8631</v>
-      </c>
-      <c r="H383" t="n">
-        <v>0</v>
-      </c>
-      <c r="I383" t="n">
-        <v>11691</v>
-      </c>
-      <c r="J383" t="n">
-        <v>7140386</v>
-      </c>
-    </row>
-    <row r="384">
-      <c r="A384" s="1" t="n">
-        <v>510</v>
-      </c>
-      <c r="B384" t="n">
-        <v>30</v>
-      </c>
-      <c r="C384" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D384" t="inlineStr">
-        <is>
-          <t>VAUPES</t>
-        </is>
-      </c>
-      <c r="E384" t="n">
-        <v>0</v>
-      </c>
-      <c r="F384" t="n">
-        <v>0</v>
-      </c>
-      <c r="G384" t="n">
-        <v>6844</v>
-      </c>
-      <c r="H384" t="n">
-        <v>0</v>
-      </c>
-      <c r="I384" t="n">
-        <v>6844</v>
-      </c>
-      <c r="J384" t="n">
-        <v>5343179</v>
-      </c>
-    </row>
-    <row r="385">
-      <c r="A385" s="1" t="n">
-        <v>511</v>
-      </c>
-      <c r="B385" t="n">
-        <v>31</v>
-      </c>
-      <c r="C385" t="inlineStr">
-        <is>
-          <t>PAPAYA</t>
-        </is>
-      </c>
-      <c r="D385" t="inlineStr">
-        <is>
-          <t>ARCHIPIELAGO DE SAN ANDRES PROVIDENCIA Y SANTA CATALINA</t>
-        </is>
-      </c>
-      <c r="E385" t="n">
-        <v>0</v>
-      </c>
-      <c r="F385" t="n">
-        <v>0</v>
-      </c>
-      <c r="G385" t="n">
-        <v>0</v>
-      </c>
-      <c r="H385" t="n">
-        <v>0</v>
-      </c>
-      <c r="I385" t="n">
-        <v>0</v>
-      </c>
-      <c r="J385" t="n">
         <v>4972</v>
       </c>
     </row>

</xml_diff>